<commit_message>
re format server code for setup manual and auto
</commit_message>
<xml_diff>
--- a/sample_files/Input_SP_Auto.xlsx
+++ b/sample_files/Input_SP_Auto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>SKU</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Percentage</t>
   </si>
   <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
     <t>set 9 - 001</t>
   </si>
   <si>
@@ -79,31 +76,22 @@
     <t>SP</t>
   </si>
   <si>
-    <t>KW</t>
-  </si>
-  <si>
-    <t>EXACT</t>
+    <t>AUTO</t>
   </si>
   <si>
     <t>Chicnchill</t>
   </si>
   <si>
-    <t xml:space="preserve">HUY </t>
-  </si>
-  <si>
-    <t>abc123,cde456</t>
-  </si>
-  <si>
-    <t>Fixed Bid</t>
+    <t>HUY</t>
+  </si>
+  <si>
+    <t>Dynamic bids - down only</t>
   </si>
   <si>
     <t>placementTop</t>
   </si>
   <si>
-    <t>ASIN</t>
-  </si>
-  <si>
-    <t>0.5,0.7</t>
+    <t>set 9 - 002</t>
   </si>
 </sst>
 </file>
@@ -113,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,26 +116,27 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,26 +151,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFc6c6c6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFc6c6c6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFc6c6c6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -189,22 +163,37 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -509,42 +498,43 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="12" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="13" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="10" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +571,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -590,148 +580,137 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="7">
+        <v>20221212</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>10</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4">
+      <c r="O2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="7">
         <v>20221212</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="7">
+        <v>2</v>
+      </c>
+      <c r="K3" s="7">
+        <v>10</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>4567</v>
-      </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="4">
-        <v>20221212</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="4">
-        <v>2</v>
-      </c>
-      <c r="K3" s="4">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>4567</v>
-      </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="P3" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>